<commit_message>
Update Tanzania data export
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict_tanzania.xlsx
+++ b/inst/extdata/day7_dict_tanzania.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="151">
   <si>
     <t>old</t>
   </si>
@@ -134,9 +134,6 @@
     <t>phonenb</t>
   </si>
   <si>
-    <t>call_ok</t>
-  </si>
-  <si>
     <t>success</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
     <t>a1-call_contact-first_attempt</t>
   </si>
   <si>
-    <t>a1-call_contact-a4_d_1a_oth</t>
-  </si>
-  <si>
     <t>a1-call_contact-respondent</t>
   </si>
   <si>
@@ -468,6 +462,21 @@
   </si>
   <si>
     <t>a1-call_contact-a4_d_1a</t>
+  </si>
+  <si>
+    <t>a1-physical_contact-meeting</t>
+  </si>
+  <si>
+    <t>successful_physical_fu</t>
+  </si>
+  <si>
+    <t>successful_phone_fu</t>
+  </si>
+  <si>
+    <t>meeting</t>
+  </si>
+  <si>
+    <t>a1-a4_d_1a_oth</t>
   </si>
 </sst>
 </file>
@@ -482,7 +491,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +534,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -538,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -565,14 +580,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,21 +872,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,7 +900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -896,7 +914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -910,7 +928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -924,7 +942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -938,7 +956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -952,676 +970,690 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>126</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>127</v>
+        <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>34</v>
+        <v>1</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="D21" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="D22" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="B23" s="9">
         <v>1</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>47</v>
+      <c r="C23" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>143</v>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>142</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" s="9">
-        <v>1</v>
-      </c>
-      <c r="C25" s="6" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
-      <c r="C26" s="6" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-      <c r="C27" s="12" t="s">
+      <c r="D28" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="5" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-      <c r="C28" s="12" t="s">
+      <c r="D29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="5" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="2">
-        <v>1</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="2">
-        <v>1</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="2">
-        <v>1</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" s="2">
-        <v>1</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" s="2">
-        <v>1</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39" s="2">
-        <v>1</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="2">
-        <v>1</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="2">
-        <v>1</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B42" s="2">
-        <v>1</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B43" s="2">
-        <v>1</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" s="2">
-        <v>1</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B46" s="2">
-        <v>1</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" s="5" t="s">
+      <c r="B48" s="2">
+        <v>1</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="2">
+        <v>1</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B47" s="2">
-        <v>1</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B48" s="2">
-        <v>1</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B49" s="2">
-        <v>1</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B50" s="2">
-        <v>1</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B52" s="2">
-        <v>1</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+      <c r="B54" s="2">
+        <v>1</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B53" s="2">
-        <v>1</v>
-      </c>
-      <c r="C53" s="6" t="s">
+      <c r="D54" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D53" s="5" t="s">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="B55" s="2">
+        <v>1</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="2">
-        <v>1</v>
-      </c>
-      <c r="C54" s="4" t="s">
+      <c r="D55" s="13" t="s">
         <v>114</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Day 7 follow-up dictionary for TZ with monitoring filter
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict_tanzania.xlsx
+++ b/inst/extdata/day7_dict_tanzania.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="152">
   <si>
     <t>old</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t>a1-a4_d_1a_oth</t>
+  </si>
+  <si>
+    <t>monitoring</t>
   </si>
 </sst>
 </file>
@@ -553,12 +556,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -567,9 +569,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -587,6 +586,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -869,787 +871,952 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="11">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="11">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="11">
         <v>0</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="11">
         <v>0</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="11">
         <v>0</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="B16" s="11">
+        <v>1</v>
+      </c>
+      <c r="C16" s="11">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="B17" s="11">
+        <v>1</v>
+      </c>
+      <c r="C17" s="11">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="11">
+        <v>1</v>
+      </c>
+      <c r="C18" s="11">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="11">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="11">
+        <v>1</v>
+      </c>
+      <c r="C20" s="11">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="E20" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9" t="s">
+      <c r="B21" s="11">
+        <v>1</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="B22" s="11">
+        <v>1</v>
+      </c>
+      <c r="C22" s="11">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B23" s="6">
-        <v>1</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="E23" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B24" s="6">
-        <v>1</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="11">
+        <v>1</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B26" s="6">
-        <v>1</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-      <c r="C27" s="9" t="s">
+      <c r="B27" s="11">
+        <v>1</v>
+      </c>
+      <c r="C27" s="11">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="B28" s="11">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29" s="8" t="s">
+      <c r="B29" s="11">
+        <v>1</v>
+      </c>
+      <c r="C29" s="11">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="E29" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="11">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11">
+        <v>1</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="2">
-        <v>1</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="11">
+        <v>1</v>
+      </c>
+      <c r="C31" s="11">
+        <v>1</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="E31" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-      <c r="C32" s="7" t="s">
+      <c r="B32" s="11">
+        <v>1</v>
+      </c>
+      <c r="C32" s="11">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="2">
-        <v>1</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="B33" s="11">
+        <v>1</v>
+      </c>
+      <c r="C33" s="11">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-      <c r="C34" s="7" t="s">
+      <c r="B34" s="11">
+        <v>1</v>
+      </c>
+      <c r="C34" s="11">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
-      <c r="C35" s="7" t="s">
+      <c r="B35" s="11">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="E35" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="2">
-        <v>1</v>
-      </c>
-      <c r="C36" s="7" t="s">
+      <c r="B36" s="11">
+        <v>1</v>
+      </c>
+      <c r="C36" s="11">
+        <v>1</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="E36" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="2">
-        <v>1</v>
-      </c>
-      <c r="C37" s="7" t="s">
+      <c r="B37" s="11">
+        <v>1</v>
+      </c>
+      <c r="C37" s="11">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="E37" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B38" s="2">
-        <v>1</v>
-      </c>
-      <c r="C38" s="7" t="s">
+      <c r="B38" s="11">
+        <v>1</v>
+      </c>
+      <c r="C38" s="11">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="2">
-        <v>1</v>
-      </c>
-      <c r="C39" s="7" t="s">
+      <c r="B39" s="11">
+        <v>1</v>
+      </c>
+      <c r="C39" s="11">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="E39" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="2">
-        <v>1</v>
-      </c>
-      <c r="C40" s="7" t="s">
+      <c r="B40" s="11">
+        <v>1</v>
+      </c>
+      <c r="C40" s="11">
+        <v>1</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="2">
-        <v>1</v>
-      </c>
-      <c r="C41" s="7" t="s">
+      <c r="B41" s="11">
+        <v>1</v>
+      </c>
+      <c r="C41" s="11">
+        <v>1</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="E41" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="2">
-        <v>1</v>
-      </c>
-      <c r="C42" s="7" t="s">
+      <c r="B42" s="11">
+        <v>1</v>
+      </c>
+      <c r="C42" s="11">
+        <v>1</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="2">
-        <v>1</v>
-      </c>
-      <c r="C43" s="7" t="s">
+      <c r="B43" s="11">
+        <v>1</v>
+      </c>
+      <c r="C43" s="11">
+        <v>1</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="E43" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-      <c r="C44" s="7" t="s">
+      <c r="B44" s="11">
+        <v>1</v>
+      </c>
+      <c r="C44" s="11">
+        <v>1</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B45" s="2">
-        <v>1</v>
-      </c>
-      <c r="C45" s="7" t="s">
+      <c r="B45" s="11">
+        <v>1</v>
+      </c>
+      <c r="C45" s="11">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="E45" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B46" s="2">
-        <v>1</v>
-      </c>
-      <c r="C46" s="7" t="s">
+      <c r="B46" s="11">
+        <v>1</v>
+      </c>
+      <c r="C46" s="11">
+        <v>1</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B47" s="2">
-        <v>1</v>
-      </c>
-      <c r="C47" s="7" t="s">
+      <c r="B47" s="11">
+        <v>1</v>
+      </c>
+      <c r="C47" s="11">
+        <v>1</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="E47" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="2">
-        <v>1</v>
-      </c>
-      <c r="C48" s="7" t="s">
+      <c r="B48" s="11">
+        <v>1</v>
+      </c>
+      <c r="C48" s="11">
+        <v>1</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="E48" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B49" s="2">
-        <v>1</v>
-      </c>
-      <c r="C49" s="7" t="s">
+      <c r="B49" s="11">
+        <v>1</v>
+      </c>
+      <c r="C49" s="11">
+        <v>1</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="E49" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="2">
-        <v>1</v>
-      </c>
-      <c r="C50" s="7" t="s">
+      <c r="B50" s="11">
+        <v>1</v>
+      </c>
+      <c r="C50" s="11">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="E50" s="8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B51" s="2">
-        <v>1</v>
-      </c>
-      <c r="C51" s="7" t="s">
+      <c r="B51" s="11">
+        <v>1</v>
+      </c>
+      <c r="C51" s="11">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="E51" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B52" s="2">
-        <v>1</v>
-      </c>
-      <c r="C52" s="7" t="s">
+      <c r="B52" s="11">
+        <v>1</v>
+      </c>
+      <c r="C52" s="11">
+        <v>1</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="E52" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B53" s="2">
-        <v>1</v>
-      </c>
-      <c r="C53" s="7" t="s">
+      <c r="B53" s="11">
+        <v>1</v>
+      </c>
+      <c r="C53" s="11">
+        <v>1</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="E53" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B54" s="2">
-        <v>1</v>
-      </c>
-      <c r="C54" s="4" t="s">
+      <c r="B54" s="11">
+        <v>1</v>
+      </c>
+      <c r="C54" s="11">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="E54" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B55" s="2">
-        <v>1</v>
-      </c>
-      <c r="C55" s="3" t="s">
+      <c r="B55" s="11">
+        <v>1</v>
+      </c>
+      <c r="C55" s="11">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="E55" s="10" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>